<commit_message>
Files updated,organized and added
</commit_message>
<xml_diff>
--- a/Files/Tables/Materials.xlsx
+++ b/Files/Tables/Materials.xlsx
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>This file will provide na overview about the properties of the materials that will be added by the mod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRUTE </t>
-  </si>
-  <si>
-    <t>REFINED</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>VALUE</t>
   </si>
@@ -37,6 +28,102 @@
   </si>
   <si>
     <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>Aetherium Shard</t>
+  </si>
+  <si>
+    <t>Adamantium Ore</t>
+  </si>
+  <si>
+    <t>Starmetal ore</t>
+  </si>
+  <si>
+    <t>Golden Sap</t>
+  </si>
+  <si>
+    <t>Purple Sap</t>
+  </si>
+  <si>
+    <t>Ferrous Salts</t>
+  </si>
+  <si>
+    <t>Manganese Ore</t>
+  </si>
+  <si>
+    <t>Nickel Ore</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Raw Spidersilk</t>
+  </si>
+  <si>
+    <t>Raw Ancestor Moth Silk</t>
+  </si>
+  <si>
+    <t>Dragon Blood</t>
+  </si>
+  <si>
+    <t>REFINED MATERIAL</t>
+  </si>
+  <si>
+    <t>BRUTE  RESOURCES</t>
+  </si>
+  <si>
+    <t>REQUIRED RESOURCES</t>
+  </si>
+  <si>
+    <t>CLASS</t>
+  </si>
+  <si>
+    <t>Produce</t>
+  </si>
+  <si>
+    <t>Rough Oak</t>
+  </si>
+  <si>
+    <t>Rough Nightwood</t>
+  </si>
+  <si>
+    <t>Rough Maple</t>
+  </si>
+  <si>
+    <t>Rough Birch</t>
+  </si>
+  <si>
+    <t>Metallic Mineral</t>
+  </si>
+  <si>
+    <t>Crystaline Mineral</t>
+  </si>
+  <si>
+    <t>Animal Material</t>
+  </si>
+  <si>
+    <t>Plant Material</t>
+  </si>
+  <si>
+    <t>Animal Product</t>
+  </si>
+  <si>
+    <t>Raw Ebonthread</t>
+  </si>
+  <si>
+    <t>Raw Akaviri Silk</t>
+  </si>
+  <si>
+    <t>Raw Cotton</t>
+  </si>
+  <si>
+    <t>Raw Ironweed</t>
+  </si>
+  <si>
+    <t>Raw Void Bloom</t>
+  </si>
+  <si>
+    <t>This file will provide an overview about the properties of the materials that will be added by the mod</t>
   </si>
 </sst>
 </file>
@@ -434,18 +521,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G7"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -453,7 +546,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -461,25 +554,212 @@
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B8:C19">
+    <sortCondition ref="C8:C19"/>
+    <sortCondition ref="B8:B19"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B2:G3"/>
   </mergeCells>

</xml_diff>